<commit_message>
Finished Welcome, Login, Gift, Shop, main menu page
</commit_message>
<xml_diff>
--- a/users database.xlsx
+++ b/users database.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\coding folder\Quizzing App\"/>
@@ -14,17 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -36,6 +31,21 @@
   </si>
   <si>
     <t>Password123@</t>
+  </si>
+  <si>
+    <t>Vsavage</t>
+  </si>
+  <si>
+    <t>Savage123@</t>
+  </si>
+  <si>
+    <t>Vandal Savage</t>
+  </si>
+  <si>
+    <t>Full name</t>
+  </si>
+  <si>
+    <t>Ude Daniel</t>
   </si>
 </sst>
 </file>
@@ -78,7 +88,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -364,32 +374,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created and added the stand alone play file
</commit_message>
<xml_diff>
--- a/users database.xlsx
+++ b/users database.xlsx
@@ -1,77 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\coding folder\Quizzing App\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>danielUde</t>
-  </si>
-  <si>
-    <t>Password123@</t>
-  </si>
-  <si>
-    <t>Vsavage</t>
-  </si>
-  <si>
-    <t>Savage123@</t>
-  </si>
-  <si>
-    <t>Vandal Savage</t>
-  </si>
-  <si>
-    <t>Full name</t>
-  </si>
-  <si>
-    <t>Ude Daniel</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -90,24 +54,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -373,56 +399,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col width="16.5703125" customWidth="1" min="1" max="1"/>
+    <col width="20.42578125" customWidth="1" min="2" max="2"/>
+    <col width="13.85546875" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Full name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>SaveMe</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">instant </t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>eliminate</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>hint</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Money</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>xp</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>danielUde</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Password123@</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Ude Daniel</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2" t="n">
+        <v>14</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3600</v>
+      </c>
+      <c r="I2" t="n">
+        <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Vsavage</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Savage123@</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Vandal Savage</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BradPitt</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BradPitt</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Brad Pitt</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BradPitt</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BradPitt123@</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Brad Pitt</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ScaJo12</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ScaJo123@</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Scarlett Johannson</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>